<commit_message>
Updated LeadPage, Lead Module, testscript
</commit_message>
<xml_diff>
--- a/Maven/src/test/resources/data/testscript.xlsx
+++ b/Maven/src/test/resources/data/testscript.xlsx
@@ -4,14 +4,15 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="7" rupBuild="4505"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2520" windowWidth="15600" windowHeight="3855"/>
+    <workbookView xWindow="0" yWindow="2520" windowWidth="15600" windowHeight="3855" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="createCampaign" sheetId="1" r:id="rId1"/>
     <sheet name="invalidLogin" sheetId="3" r:id="rId2"/>
+    <sheet name="createLead" sheetId="4" r:id="rId3"/>
   </sheets>
   <calcPr calcId="124519"/>
-  <oleSize ref="A1:N11"/>
+  <oleSize ref="A1:P11"/>
   <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
     <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -21,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="36">
   <si>
     <t>Sl.No</t>
   </si>
@@ -105,6 +106,30 @@
   </si>
   <si>
     <t>ExpectedResponse</t>
+  </si>
+  <si>
+    <t>FirstName</t>
+  </si>
+  <si>
+    <t>LastName</t>
+  </si>
+  <si>
+    <t>Company</t>
+  </si>
+  <si>
+    <t>LeadSource</t>
+  </si>
+  <si>
+    <t>Prafull</t>
+  </si>
+  <si>
+    <t>Ullagedde</t>
+  </si>
+  <si>
+    <t>Sobha</t>
+  </si>
+  <si>
+    <t>Advertisement</t>
   </si>
 </sst>
 </file>
@@ -453,7 +478,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -463,7 +488,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:K2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
@@ -652,4 +677,58 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:E2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="2" max="2" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C1" t="s">
+        <v>29</v>
+      </c>
+      <c r="D1" t="s">
+        <v>30</v>
+      </c>
+      <c r="E1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C2" t="s">
+        <v>33</v>
+      </c>
+      <c r="D2" t="s">
+        <v>34</v>
+      </c>
+      <c r="E2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>